<commit_message>
spreadsheets: Bug fix; cost_of_activities cost_of_activities was missing amount
</commit_message>
<xml_diff>
--- a/indigo/spreadsheetform_guides/project_public_v006.xlsx
+++ b/indigo/spreadsheetform_guides/project_public_v006.xlsx
@@ -1448,7 +1448,7 @@
     <t xml:space="preserve">SPREADSHEETFORM:DOWN:technical_assistance_details:cost_type/value</t>
   </si>
   <si>
-    <t xml:space="preserve">SPREADSHEETFORM:DOWN:technical_assistance_details:cost_of_activities/value</t>
+    <t xml:space="preserve">SPREADSHEETFORM:DOWN:technical_assistance_details:cost_of_activities/amount/value</t>
   </si>
   <si>
     <t xml:space="preserve">SPREADSHEETFORM:DOWN:technical_assistance_details:number_of_days/value</t>
@@ -4853,7 +4853,7 @@
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="53.91"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="23.2"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="50.15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="50.14"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="4" style="0" width="11.52"/>
   </cols>
   <sheetData>

</xml_diff>